<commit_message>
Tabulated the pseudo code
</commit_message>
<xml_diff>
--- a/Pseudo Code/CalcMatch.xlsx
+++ b/Pseudo Code/CalcMatch.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
   <si>
     <t>Name: Type</t>
   </si>
@@ -80,15 +80,9 @@
     <t xml:space="preserve">begin if </t>
   </si>
   <si>
-    <t xml:space="preserve">totalTeamScoreA = totalTeamScoreB </t>
-  </si>
-  <si>
     <t xml:space="preserve">end if </t>
   </si>
   <si>
-    <t>teamAscore &gt; teambBScore</t>
-  </si>
-  <si>
     <t>(teamaScore + randTeamScoreA)/10 = totalTeamScoreA</t>
   </si>
   <si>
@@ -101,24 +95,9 @@
     <t>\\calculate losers score</t>
   </si>
   <si>
-    <t>goalKeeperScore= get winning teams goalkeeper attribute add random 1-10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">attackScore = get loser teams attak and random 1-10 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">goalKeeperScore - attackScore &gt; 0 </t>
-  </si>
-  <si>
     <t xml:space="preserve">rounded up </t>
   </si>
   <si>
-    <t>then LoserScore = (goalKepperScore-attackScore)/2</t>
-  </si>
-  <si>
-    <t>TeamteamAScore - teamBScore = WinnerScore</t>
-  </si>
-  <si>
     <t>WinnerScore int</t>
   </si>
   <si>
@@ -128,16 +107,37 @@
     <t>CalculateMatch()</t>
   </si>
   <si>
-    <t>then randDrawScore = winnerGoalScore</t>
-  </si>
-  <si>
-    <t>winnerGoalScore = loserGoalScore</t>
-  </si>
-  <si>
     <t>Pseudo Code</t>
   </si>
   <si>
     <t>calculateResults(getFixtureID(),teamAScore int, teamBScore int) \\team A will always be the home team</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    totalTeamScoreA = totalTeamScoreB </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    then randDrawScore = winnerGoalScore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    winnerGoalScore = loserGoalScore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    teamAscore &gt; teambBScore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    goalKeeperScore= get winning teams goalkeeper attribute add random 1-10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    attackScore = get loser teams attak and random 1-10 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    then TeamteamAScore - teamBScore = WinnerScore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    goalKeeperScore - attackScore &gt; 0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    then LoserScore = (goalKepperScore-attackScore)/2</t>
   </si>
 </sst>
 </file>
@@ -239,10 +239,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -549,8 +549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -561,15 +561,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="8"/>
-      <c r="B1" s="8"/>
+      <c r="A1" s="9"/>
+      <c r="B1" s="9"/>
     </row>
     <row r="2" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
@@ -627,13 +627,13 @@
     <row r="13" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="5" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
       <c r="B14" s="4" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
@@ -662,7 +662,7 @@
     </row>
     <row r="20" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
-      <c r="B20" s="5"/>
+      <c r="B20" s="4"/>
     </row>
     <row r="21" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
@@ -747,13 +747,13 @@
     <row r="36" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A36" s="2"/>
       <c r="B36" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A37" s="2"/>
       <c r="B37" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
@@ -765,25 +765,25 @@
     <row r="39" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A39" s="2"/>
       <c r="B39" s="4" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A40" s="2"/>
       <c r="B40" s="4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A41" s="2"/>
       <c r="B41" s="4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A42" s="2"/>
       <c r="B42" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
@@ -794,67 +794,69 @@
     </row>
     <row r="44" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A45" s="2"/>
       <c r="B45" s="4" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A47" s="2"/>
       <c r="B47" s="4" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A48" s="2"/>
       <c r="B48" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A49" s="2"/>
       <c r="B49" s="4" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A51" s="2"/>
       <c r="B51" s="4" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A52" s="2"/>
-      <c r="B52" s="9" t="s">
-        <v>38</v>
+      <c r="B52" s="4" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A53" s="2"/>
-      <c r="B53" s="4"/>
+      <c r="B53" s="8" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="54" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A54" s="2"/>

</xml_diff>